<commit_message>
supermarkety-only-obyv.xlsx - označeny okresní města
</commit_message>
<xml_diff>
--- a/data/supermarkety-only-obyv.xlsx
+++ b/data/supermarkety-only-obyv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="supermarkety-only-obyv" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
     <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -11956,7 +11956,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12142,6 +12142,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -12303,7 +12309,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -12313,6 +12319,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -12358,7 +12370,709 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -41354,7 +42068,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:O151" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -42031,6 +42745,481 @@
     <dataField name="Sum of SUMOBZSJ01" fld="6" showDataAs="percentOfRow" baseField="1" baseItem="0" numFmtId="10"/>
     <dataField name="Count of FIRMA" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="50">
+    <format dxfId="100">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="98">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="97">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="96">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="95">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="94">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="3">
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="93">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="92">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="15"/>
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="91">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="90">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="22"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="89">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="88">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="27"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="87">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="30"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="86">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="34"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="85">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="38"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="84">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="41"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="83">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="82">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="46"/>
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="81">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="3">
+            <x v="49"/>
+            <x v="50"/>
+            <x v="51"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="80">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="53"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="79">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="3">
+            <x v="54"/>
+            <x v="55"/>
+            <x v="56"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="78">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="62"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="77">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="65"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="76">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="68"/>
+            <x v="69"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="75">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="71"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="73"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="75"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="77"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="78"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="70">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="80"/>
+            <x v="81"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="83"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="68">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="84"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="86"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="66">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="88"/>
+            <x v="89"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="91"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="93"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="3">
+            <x v="94"/>
+            <x v="95"/>
+            <x v="96"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="4">
+            <x v="99"/>
+            <x v="100"/>
+            <x v="101"/>
+            <x v="102"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="105"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="108"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="59">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="110"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="112"/>
+            <x v="113"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="57">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="116"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="56">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="3">
+            <x v="117"/>
+            <x v="118"/>
+            <x v="119"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="55">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="122"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="54">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="124"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="53">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="128"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="52">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="130"/>
+            <x v="131"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="51">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="4">
+            <x v="138"/>
+            <x v="139"/>
+            <x v="140"/>
+            <x v="141"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="50">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="143"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -91095,7 +92284,7 @@
   <dimension ref="A3:O151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -91178,7 +92367,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="5">
@@ -91225,7 +92414,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="8" t="s">
         <v>114</v>
       </c>
       <c r="B7" s="5">
@@ -91272,7 +92461,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B8" s="5">
@@ -91319,7 +92508,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5">
@@ -91366,7 +92555,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="8" t="s">
         <v>442</v>
       </c>
       <c r="B10" s="5">
@@ -91413,7 +92602,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="8" t="s">
         <v>132</v>
       </c>
       <c r="B11" s="5">
@@ -91460,7 +92649,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="8" t="s">
         <v>88</v>
       </c>
       <c r="B12" s="5">
@@ -91507,7 +92696,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="8" t="s">
         <v>193</v>
       </c>
       <c r="B13" s="5">
@@ -91552,7 +92741,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="8" t="s">
         <v>219</v>
       </c>
       <c r="B14" s="5">
@@ -91599,7 +92788,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="8" t="s">
         <v>699</v>
       </c>
       <c r="B15" s="5">
@@ -91646,7 +92835,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B16" s="5">
@@ -91693,7 +92882,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="8" t="s">
         <v>513</v>
       </c>
       <c r="B17" s="5">
@@ -91740,7 +92929,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="5">
@@ -91787,7 +92976,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="5">
@@ -91834,7 +93023,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="8" t="s">
         <v>359</v>
       </c>
       <c r="B20" s="5">
@@ -91881,7 +93070,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="8" t="s">
         <v>305</v>
       </c>
       <c r="B21" s="5">
@@ -91926,7 +93115,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5">
@@ -91973,7 +93162,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="5">
@@ -92020,7 +93209,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="8" t="s">
         <v>625</v>
       </c>
       <c r="B24" s="5">
@@ -92065,7 +93254,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="8" t="s">
         <v>869</v>
       </c>
       <c r="B25" s="5">
@@ -92110,7 +93299,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="8" t="s">
         <v>571</v>
       </c>
       <c r="B26" s="5">
@@ -92157,7 +93346,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="8" t="s">
         <v>424</v>
       </c>
       <c r="B27" s="5">
@@ -92204,7 +93393,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="8" t="s">
         <v>368</v>
       </c>
       <c r="B28" s="5">
@@ -92251,7 +93440,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="8" t="s">
         <v>188</v>
       </c>
       <c r="B29" s="5">
@@ -92298,7 +93487,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="8" t="s">
         <v>1433</v>
       </c>
       <c r="B30" s="5">
@@ -92345,7 +93534,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="8" t="s">
         <v>206</v>
       </c>
       <c r="B31" s="5">
@@ -92392,7 +93581,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="8" t="s">
         <v>1420</v>
       </c>
       <c r="B32" s="5">
@@ -92437,7 +93626,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="8" t="s">
         <v>753</v>
       </c>
       <c r="B33" s="5">
@@ -92482,7 +93671,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="8" t="s">
         <v>556</v>
       </c>
       <c r="B34" s="5">
@@ -92529,7 +93718,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="8" t="s">
         <v>250</v>
       </c>
       <c r="B35" s="5">
@@ -92574,7 +93763,7 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="8" t="s">
         <v>310</v>
       </c>
       <c r="B36" s="5">
@@ -92621,7 +93810,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="8" t="s">
         <v>233</v>
       </c>
       <c r="B37" s="5">
@@ -92668,7 +93857,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="8" t="s">
         <v>472</v>
       </c>
       <c r="B38" s="5">
@@ -92715,7 +93904,7 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="8" t="s">
         <v>104</v>
       </c>
       <c r="B39" s="5">
@@ -92760,7 +93949,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="8" t="s">
         <v>935</v>
       </c>
       <c r="B40" s="5">
@@ -92805,7 +93994,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="8" t="s">
         <v>377</v>
       </c>
       <c r="B41" s="5">
@@ -92848,7 +94037,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="8" t="s">
         <v>228</v>
       </c>
       <c r="B42" s="5">
@@ -92895,7 +94084,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="8" t="s">
         <v>166</v>
       </c>
       <c r="B43" s="5">
@@ -92940,7 +94129,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="8" t="s">
         <v>1860</v>
       </c>
       <c r="B44" s="5">
@@ -92983,7 +94172,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B45" s="5">
@@ -93028,7 +94217,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="8" t="s">
         <v>535</v>
       </c>
       <c r="B46" s="5">
@@ -93075,7 +94264,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="8" t="s">
         <v>1073</v>
       </c>
       <c r="B47" s="5">
@@ -93120,7 +94309,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="8" t="s">
         <v>1316</v>
       </c>
       <c r="B48" s="5">
@@ -93165,7 +94354,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="8" t="s">
         <v>882</v>
       </c>
       <c r="B49" s="5">
@@ -93210,7 +94399,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="8" t="s">
         <v>969</v>
       </c>
       <c r="B50" s="5">
@@ -93255,7 +94444,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="8" t="s">
         <v>354</v>
       </c>
       <c r="B51" s="5">
@@ -93298,7 +94487,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="8" t="s">
         <v>671</v>
       </c>
       <c r="B52" s="5">
@@ -93341,7 +94530,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="8" t="s">
         <v>1151</v>
       </c>
       <c r="B53" s="5">
@@ -93384,7 +94573,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="8" t="s">
         <v>662</v>
       </c>
       <c r="B54" s="5">
@@ -93429,7 +94618,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="8" t="s">
         <v>171</v>
       </c>
       <c r="B55" s="5">
@@ -93474,7 +94663,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="8" t="s">
         <v>292</v>
       </c>
       <c r="B56" s="5">
@@ -93519,7 +94708,7 @@
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="8" t="s">
         <v>1231</v>
       </c>
       <c r="B57" s="5">
@@ -93562,7 +94751,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="8" t="s">
         <v>398</v>
       </c>
       <c r="B58" s="5">
@@ -93607,7 +94796,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="8" t="s">
         <v>149</v>
       </c>
       <c r="B59" s="5">
@@ -93650,7 +94839,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="8" t="s">
         <v>526</v>
       </c>
       <c r="B60" s="5">
@@ -93691,7 +94880,7 @@
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="8" t="s">
         <v>1562</v>
       </c>
       <c r="B61" s="5">
@@ -93736,7 +94925,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="8" t="s">
         <v>93</v>
       </c>
       <c r="B62" s="5">
@@ -93781,7 +94970,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B63" s="5">
@@ -93824,7 +95013,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="8" t="s">
         <v>1868</v>
       </c>
       <c r="B64" s="5">
@@ -93867,7 +95056,7 @@
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="8" t="s">
         <v>952</v>
       </c>
       <c r="B65" s="5">
@@ -93910,7 +95099,7 @@
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="8" t="s">
         <v>287</v>
       </c>
       <c r="B66" s="5">
@@ -93955,7 +95144,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="8" t="s">
         <v>429</v>
       </c>
       <c r="B67" s="5">
@@ -94000,7 +95189,7 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="8" t="s">
         <v>297</v>
       </c>
       <c r="B68" s="5">
@@ -94043,7 +95232,7 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="8" t="s">
         <v>1691</v>
       </c>
       <c r="B69" s="5">
@@ -94086,7 +95275,7 @@
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="8" t="s">
         <v>333</v>
       </c>
       <c r="B70" s="5">
@@ -94129,7 +95318,7 @@
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="8" t="s">
         <v>592</v>
       </c>
       <c r="B71" s="5">
@@ -94172,7 +95361,7 @@
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="8" t="s">
         <v>323</v>
       </c>
       <c r="B72" s="5">
@@ -94215,7 +95404,7 @@
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="8" t="s">
         <v>99</v>
       </c>
       <c r="B73" s="5">
@@ -94256,7 +95445,7 @@
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="7" t="s">
         <v>630</v>
       </c>
       <c r="B74" s="5">
@@ -94299,7 +95488,7 @@
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="8" t="s">
         <v>1499</v>
       </c>
       <c r="B75" s="5">
@@ -94502,7 +95691,7 @@
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="8" t="s">
         <v>1627</v>
       </c>
       <c r="B80" s="5">
@@ -97205,5 +98394,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>